<commit_message>
fix pytest run command
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -90,7 +90,7 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
-    <t xml:space="preserve">uni142001@gmail.com</t>
+    <t xml:space="preserve">uni132001@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Check success register</t>
@@ -334,7 +334,7 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>